<commit_message>
add aboutUs & settings
</commit_message>
<xml_diff>
--- a/doc/driver.xlsx
+++ b/doc/driver.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168">
   <si>
     <t>模块</t>
   </si>
@@ -588,24 +588,6 @@
   <si>
     <t>访问频繁</t>
   </si>
-  <si>
-    <t>设备接口明细</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. 获取司机连接的设备wifi的公司名称   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. 获取设备当前上网用户人数     </t>
-  </si>
-  <si>
-    <t>1. 获取设备当前车辆信息</t>
-  </si>
-  <si>
-    <t>1. 设备日检 获取设备 车牌号、SN、WIFI连接、Portal页面等检测信息</t>
-  </si>
-  <si>
-    <t>1. 获取设备位置信息lat lng</t>
-  </si>
 </sst>
 </file>
 
@@ -614,8 +596,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -643,20 +625,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -671,11 +639,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -686,19 +654,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -717,37 +708,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -755,10 +715,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -777,30 +737,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,12 +813,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -851,13 +921,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -869,145 +975,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1045,11 +1019,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1083,8 +1063,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1104,169 +1084,163 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1313,10 +1287,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="32" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1668,7 +1639,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B66:B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.15" customHeight="1"/>
@@ -2689,40 +2660,28 @@
       </c>
     </row>
     <row r="66" customHeight="1" spans="2:3">
-      <c r="B66" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="C66" s="17"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
     </row>
     <row r="67" customHeight="1" spans="2:3">
-      <c r="B67" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C67" s="17"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
     </row>
     <row r="68" customHeight="1" spans="2:3">
-      <c r="B68" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="C68" s="17"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
     </row>
     <row r="69" customHeight="1" spans="2:3">
-      <c r="B69" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="C69" s="17"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
     </row>
     <row r="70" customHeight="1" spans="2:3">
-      <c r="B70" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C70" s="17"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
     </row>
     <row r="71" customHeight="1" spans="2:3">
-      <c r="B71" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="C71" s="17"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:B64">

</xml_diff>